<commit_message>
set resource id for each element
</commit_message>
<xml_diff>
--- a/MMAPlus_Merchandising/MMA_Merchandising.xlsx
+++ b/MMAPlus_Merchandising/MMA_Merchandising.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EC9A4D-77F0-4D5B-A9E1-A0CAFA87EC7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08515226-3FF2-4CF9-B835-B2BF9B3B259F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{65B03DFA-846A-4EE9-BFD9-C2885113F2BF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{65B03DFA-846A-4EE9-BFD9-C2885113F2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Distribution Point" sheetId="11" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7220" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7221" uniqueCount="224">
   <si>
     <t>Flavoured Milk</t>
   </si>
@@ -691,6 +691,9 @@
   </si>
   <si>
     <t>Merchandiser Scores</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
@@ -1472,7 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T1128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -62441,11 +62444,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC505BDA-4272-4758-9DA2-F72D83B99B5B}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62518,6 +62521,11 @@
         <v>220</v>
       </c>
     </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>223</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>